<commit_message>
DaoNgocHung - Thêm code project
</commit_message>
<xml_diff>
--- a/Ý tưởng/Demo_Database.xlsx
+++ b/Ý tưởng/Demo_Database.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TLCN_LATN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TLCN_LATN\Git\GreenBook\Ý tưởng\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Table_Book" sheetId="1" r:id="rId1"/>
-    <sheet name="Table_Author" sheetId="4" r:id="rId2"/>
-    <sheet name="Table_Category" sheetId="5" r:id="rId3"/>
-    <sheet name="Table_User" sheetId="3" r:id="rId4"/>
-    <sheet name="Table_Comment" sheetId="2" r:id="rId5"/>
+    <sheet name="Book" sheetId="1" r:id="rId1"/>
+    <sheet name="Author" sheetId="4" r:id="rId2"/>
+    <sheet name="Category" sheetId="5" r:id="rId3"/>
+    <sheet name="User" sheetId="3" r:id="rId4"/>
+    <sheet name="Comment" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
   <si>
     <t>Thuộc tính</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Dùng để lưu số lần nhập sai mật khẩu của tài khoản. Nếu nhập sai 5 lần thì tài khoản bị vô hịu hóa. Nếu nhập  đúng thì sẽ reset về 0</t>
+  </si>
+  <si>
+    <t>ID_User</t>
+  </si>
+  <si>
+    <t>ID tài khoản</t>
   </si>
 </sst>
 </file>
@@ -952,10 +958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,10 +986,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +997,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,10 +1008,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,10 +1019,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,10 +1030,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,10 +1041,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1052,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,10 +1063,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1068,10 +1074,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,10 +1085,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,10 +1096,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,9 +1107,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>79</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1116,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>